<commit_message>
finalizando modulo de red
</commit_message>
<xml_diff>
--- a/Ciberseguridad.xlsx
+++ b/Ciberseguridad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Biblioteca\Escritorio\Ciberseguridad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6047DFE-17F5-41E9-8893-861A6CE1E1F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B941C915-B721-425D-923A-D2502F7A659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="1373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="1404">
   <si>
     <t>Forense</t>
   </si>
@@ -7214,6 +7214,126 @@
   </si>
   <si>
     <t>Phase 2. Vulnerability Scanning and Analysis</t>
+  </si>
+  <si>
+    <t>Evasion and persistence</t>
+  </si>
+  <si>
+    <t>Meterpreter es una herramienta avanzada de post-explotación utilizada en pruebas de penetración y auditorías de seguridad. Es un payload (código malicioso) que se inyecta en un sistema comprometido para proporcionar al atacante un control interactivo y flexible sobre ese sistema. Meterpreter forma parte del framework Metasploit, muy popular en el ámbito de la seguridad informática.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSFVENOM </t>
+  </si>
+  <si>
+    <t>Post explotacion / Metasploit</t>
+  </si>
+  <si>
+    <t>Msfvenom es una herramienta del framework Metasploit que se utiliza para generar payloads personalizados para pruebas de penetración. Combina las funciones de las antiguas herramientas msfpayload y msfencode, permitiendo crear código malicioso (payloads) que se puede inyectar en sistemas objetivo para obtener acceso o ejecutar comandos.
+Con msfvenom puedes elegir el tipo de payload, el formato de salida (por ejemplo, ejecutables, scripts, código en varios lenguajes), y aplicar técnicas de codificación para evadir detección por antivirus. Es muy útil para preparar ataques controlados y autorizados en un entorno de pentesting.</t>
+  </si>
+  <si>
+    <t>Telnet</t>
+  </si>
+  <si>
+    <t>El comando telnet en Linux se utiliza para conectarse a un servidor remoto a través del protocolo Telnet, que permite acceder a una interfaz de línea de comandos en ese servidor. Principalmente, se usa para probar la conectividad a un puerto específico de un servidor, diagnosticar problemas de red o acceder a dispositivos que soportan Telnet.
+Sin embargo, Telnet no cifra la comunicación, por lo que no es seguro para conexiones sensibles; hoy en día se prefiere usar SSH para acceso remoto seguro. //  écnicamente Telnet podría usarse como un canal de comando y control (C2) en un entorno de pruebas o simulaciones, porque permite enviar comandos a un sistema remoto y recibir respuestas. Sin embargo, debido a que Telnet no cifra la comunicación y es fácilmente detectable, no es una opción práctica ni segura para un C2 real en ataques sofisticados.</t>
+  </si>
+  <si>
+    <r>
+      <t>smtp-user-enum -M VRFY -u [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>usuario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>] -t 192.168.78.8</t>
+    </r>
+  </si>
+  <si>
+    <t>verificar si el usuario existe en el servidor.</t>
+  </si>
+  <si>
+    <t>VRFY y EXPN</t>
+  </si>
+  <si>
+    <t>EMPIRE</t>
+  </si>
+  <si>
+    <t>C2 Comand and Control</t>
+  </si>
+  <si>
+    <t>Empire Framework es una herramienta de post-explotación utilizada principalmente en pruebas de penetración y auditorías de seguridad. Sirve para controlar de manera remota sistemas comprometidos mediante agentes que se ejecutan en las máquinas objetivo. Permite a los pentesters ejecutar comandos, cargar módulos, realizar movimientos laterales, recolectar información y mantener acceso persistente en entornos Windows, Linux y macOS. Es muy valorada por su capacidad para evadir detecciones y su flexibilidad en ataques avanzados.</t>
+  </si>
+  <si>
+    <t>C2 Command and Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2 Command and Control / movimientos laterales / evasión y persistencia </t>
+  </si>
+  <si>
+    <t>schtasks.exe</t>
+  </si>
+  <si>
+    <t>Con schtasks.exe, un atacante o un pentester autorizado puede abusar de esta herramienta para crear tareas programadas maliciosas que se ejecutarán automáticamente, lo que facilita la persistencia en un sistema comprometido. Por ejemplo, se puede usar para ejecutar malware, scripts de recolección de información, o comandos maliciosos en intervalos regulares o al iniciar sesión, sin necesidad de interacción directa.</t>
+  </si>
+  <si>
+    <t>Privilege Escalation</t>
+  </si>
+  <si>
+    <t>Consola Windows</t>
+  </si>
+  <si>
+    <t>C2 Command and Control sin cifrado</t>
+  </si>
+  <si>
+    <t>Attacks on operating systems (Privilege Escalation)</t>
+  </si>
+  <si>
+    <t>Kerberoasting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kerberoasting es una técnica de ataque en entornos Windows basada en Active Directory que permite a un atacante obtener hashes de contraseñas de cuentas de servicio con permisos elevados. El atacante solicita tickets de servicio (TGS) para estas cuentas, que están cifrados con la contraseña del servicio, y luego extrae esos tickets para intentar crackearlos sin conexión y obtener la contraseña en texto claro.
+Este ataque es peligroso porque no requiere privilegios elevados para iniciarlo; un usuario autenticado normal puede solicitar estos tickets. Una vez que el atacante obtiene la contraseña una cuenta de servicio, puede usarla para moverse lateralmente o escalar privilegios dentro de la red.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impacket  // Rubeus </t>
+  </si>
+  <si>
+    <t>Bettercap</t>
+  </si>
+  <si>
+    <t>Cain y abel</t>
+  </si>
+  <si>
+    <t>Mitmframwork</t>
+  </si>
+  <si>
+    <t>Arpspoof</t>
+  </si>
+  <si>
+    <t>Fluxion</t>
+  </si>
+  <si>
+    <t>Marco de reconocimiento y explotación de redes tanto cableadas como inalámbricas</t>
+  </si>
+  <si>
+    <t>Network and service attacks</t>
   </si>
 </sst>
 </file>
@@ -15914,256 +16034,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>690838</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>175058</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>5041</xdr:rowOff>
+      <xdr:rowOff>18116</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>477927</xdr:colOff>
-      <xdr:row>106</xdr:row>
-      <xdr:rowOff>105895</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectángulo: esquinas redondeadas 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{230302C4-246E-44BF-B8AA-984425EB0B06}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13644838" y="15054541"/>
-          <a:ext cx="2835089" cy="5244354"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Ataques y explotaciones basados en la resolución de nombres de Windows</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Ataque de envenenamiento de caché DNS</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Ataques y explotaciones contra implementaciones de Server Message Block (SMB)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Vulnerabilidades y explotaciones del Protocolo simple de administración de red (SNMP)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Vulnerabilidades y explotaciones del Protocolo simple de transferencia de correo (SMTP)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Vulnerabilidades y explotaciones del Protocolo de transferencia de archivos (FTP)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Ataques de transferencia de hash</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Ataques en ruta (antes conocidos como ataques de intermediario [MITM])</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Ataques de eliminación de SSL</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Ataques de denegación de servicio (DoS) y de denegación de servicio distribuido (DDoS)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Omisión del control de acceso a la red (NAC)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>-Ataques de salto a la red de área local virtual (VLAN)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-CO" sz="1100" b="1" i="0" u="none">
-            <a:solidFill>
-              <a:schemeClr val="lt1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>289358</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>37166</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>17369</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>658906</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>188819</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -16178,7 +16058,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14005358" y="20801666"/>
+          <a:off x="13891058" y="15067616"/>
           <a:ext cx="2007848" cy="932703"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -16316,15 +16196,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>302558</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>62193</xdr:rowOff>
+      <xdr:colOff>207308</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>14568</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>750794</xdr:colOff>
-      <xdr:row>120</xdr:row>
-      <xdr:rowOff>42396</xdr:rowOff>
+      <xdr:colOff>655544</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>185271</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -16339,7 +16219,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14018558" y="21969693"/>
+          <a:off x="13923308" y="16207068"/>
           <a:ext cx="1972236" cy="932703"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -16469,15 +16349,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>302559</xdr:colOff>
-      <xdr:row>121</xdr:row>
-      <xdr:rowOff>46505</xdr:rowOff>
+      <xdr:colOff>197784</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>189380</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>17928</xdr:colOff>
-      <xdr:row>126</xdr:row>
-      <xdr:rowOff>26708</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>675153</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>169583</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -16492,7 +16372,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14018559" y="23097005"/>
+          <a:off x="13913784" y="17334380"/>
           <a:ext cx="2001369" cy="932703"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -16551,7 +16431,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Explotacion  SNMP puerto 161 (phishing - correos )</a:t>
+            <a:t>Explotacion  SNMP puerto TCP 25, 465, 587, 110, 995, 143, 993 (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>administrar dispositivos de red</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
             <a:solidFill>
@@ -17074,14 +16978,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>28576</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>666751</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>200026</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
@@ -17098,8 +17002,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13744576" y="8562975"/>
-          <a:ext cx="2457450" cy="1466850"/>
+          <a:off x="13620751" y="8562975"/>
+          <a:ext cx="2686049" cy="1466850"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -17250,7 +17154,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>- Envenenamiento de caché                      - Envenenamiento LLMNR/NBT-NS</a:t>
+            <a:t>- Envenenamiento de caché                     </a:t>
           </a:r>
           <a:br>
             <a:rPr lang="es-CO" sz="1100" b="0" i="0" baseline="0">
@@ -17273,7 +17177,125 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>- Ataque de degradación</a:t>
+            <a:t> - Envenenamiento LLMNR/NBT-NS</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Ataque de degradación (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>POODLE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Ettercap -</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Be</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ttercap </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
           </a:r>
           <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
             <a:solidFill>
@@ -18270,6 +18292,1085 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>705969</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>170703</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rectángulo: esquinas redondeadas 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84B5E5CC-46EC-4873-A11D-E64A7BC00ABD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13944600" y="18478500"/>
+          <a:ext cx="2001369" cy="932703"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Explotacion SMTP </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(Correos - Phising) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>comandos </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>VRFY</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> y </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>EXPN</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>686919</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>132603</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rectángulo: esquinas redondeadas 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97E11128-8019-40C9-B60D-8994156D9843}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13925550" y="19583400"/>
+          <a:ext cx="2001369" cy="932703"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Explotacion  FTP puerto 21</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>705969</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>151653</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Rectángulo: esquinas redondeadas 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA3FF551-B7A7-474C-87CC-0EB099979442}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13944600" y="20745450"/>
+          <a:ext cx="2001369" cy="932703"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Ataques de tipo Pass-the-Hash.  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Administrador de cuentas de seguridad (SAM) (Mimikatz para</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> windows</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>705969</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>189753</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectángulo: esquinas redondeadas 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E84A39D-F0C8-4B73-83FC-75E97561040A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13944600" y="21926550"/>
+          <a:ext cx="2001369" cy="932703"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Ataques basados ​​en Kerberos y LDAP (Mimikatz - empire</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> framwork - starkiller</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>715494</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>189753</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Rectángulo: esquinas redondeadas 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82EA8750-2291-47A4-B4AB-66751DA4F08E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13954125" y="23069550"/>
+          <a:ext cx="2001369" cy="932703"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Ataque Kerberoasting (Impacket</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Rubeus)</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>753594</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>189753</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Rectángulo: esquinas redondeadas 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99192449-77DE-4543-BCE2-803D7B8C06E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13992225" y="24212550"/>
+          <a:ext cx="2001369" cy="932703"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Ataques de manipulación de rutas (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Border Gateway Protocol (BGP)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>20169</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>189753</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Rectángulo: esquinas redondeadas 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19E568C5-3B63-413E-BB66-AA8E3C0003B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14020800" y="25355550"/>
+          <a:ext cx="2001369" cy="932703"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Omisión del control de acceso a la red (NAC)</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1119</xdr:colOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>170703</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="37" name="Rectángulo: esquinas redondeadas 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92F05008-829C-452F-BA3B-EAE27A881116}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14001750" y="26479500"/>
+          <a:ext cx="2001369" cy="932703"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Saltos de (VLAN)</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>39219</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>161178</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="Rectángulo: esquinas redondeadas 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B78CC5B-3E0C-4362-A8E5-0287BF19B8B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14039850" y="27612975"/>
+          <a:ext cx="2001369" cy="932703"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1100" b="1" i="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Ataques de inanición de DHCP y servidores DHCP no autorizados</a:t>
+          </a:r>
+          <a:endParaRPr lang="es-CO" sz="1100" b="0" i="0">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -19725,15 +20826,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H300"/>
   <sheetViews>
-    <sheetView topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A220" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D228" sqref="D228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" style="81" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="81" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="50.140625" customWidth="1"/>
     <col min="6" max="6" width="42.5703125" customWidth="1"/>
@@ -24348,7 +25449,9 @@
         <v>3</v>
       </c>
       <c r="B218" s="3"/>
-      <c r="C218" s="80"/>
+      <c r="C218" s="87" t="s">
+        <v>1384</v>
+      </c>
       <c r="D218" s="3" t="s">
         <v>107</v>
       </c>
@@ -24360,26 +25463,36 @@
       </c>
       <c r="H218" s="4"/>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" ht="60">
       <c r="A219" s="3">
         <v>3</v>
       </c>
       <c r="B219" s="3"/>
-      <c r="C219" s="80"/>
-      <c r="E219" s="48" t="s">
+      <c r="C219" s="87" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D219" s="51" t="s">
+        <v>944</v>
+      </c>
+      <c r="E219" s="51" t="s">
         <v>1347</v>
       </c>
       <c r="F219" s="3" t="s">
         <v>1346</v>
       </c>
-      <c r="H219" s="4"/>
+      <c r="G219" s="3"/>
+      <c r="H219" s="4" t="s">
+        <v>1374</v>
+      </c>
     </row>
     <row r="220" spans="1:8" ht="105">
       <c r="A220" s="3">
         <v>3</v>
       </c>
       <c r="B220" s="3"/>
-      <c r="C220" s="80"/>
+      <c r="C220" s="87" t="s">
+        <v>1403</v>
+      </c>
       <c r="D220" s="3" t="s">
         <v>107</v>
       </c>
@@ -24414,134 +25527,273 @@
       <c r="G221" s="3" t="s">
         <v>1364</v>
       </c>
-    </row>
-    <row r="222" spans="1:8">
+      <c r="H221" s="99"/>
+    </row>
+    <row r="222" spans="1:8" ht="105">
       <c r="A222" s="3">
         <v>3</v>
       </c>
       <c r="B222" s="3"/>
-      <c r="C222" s="80"/>
-    </row>
-    <row r="223" spans="1:8">
+      <c r="C222" s="87" t="s">
+        <v>1373</v>
+      </c>
+      <c r="D222" s="51" t="s">
+        <v>944</v>
+      </c>
+      <c r="E222" s="51" t="s">
+        <v>1376</v>
+      </c>
+      <c r="F222" s="3" t="s">
+        <v>1375</v>
+      </c>
+      <c r="H222" s="99" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" ht="120">
       <c r="A223" s="3">
         <v>3</v>
       </c>
       <c r="B223" s="3"/>
-      <c r="C223" s="80"/>
+      <c r="C223" s="83" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D223" s="51" t="s">
+        <v>944</v>
+      </c>
+      <c r="E223" s="51" t="s">
+        <v>1392</v>
+      </c>
+      <c r="F223" s="3" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H223" s="99" t="s">
+        <v>1379</v>
+      </c>
     </row>
     <row r="224" spans="1:8">
       <c r="A224" s="3">
         <v>3</v>
       </c>
       <c r="B224" s="3"/>
-      <c r="C224" s="80"/>
-    </row>
-    <row r="225" spans="1:3">
+      <c r="C224" s="83" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D224" s="51" t="s">
+        <v>944</v>
+      </c>
+      <c r="E224" s="51"/>
+      <c r="F224" s="3" t="s">
+        <v>1382</v>
+      </c>
+      <c r="G224" s="1" t="s">
+        <v>1380</v>
+      </c>
+      <c r="H224" s="99" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" ht="75">
       <c r="A225" s="3">
         <v>3</v>
       </c>
       <c r="B225" s="3"/>
-      <c r="C225" s="80"/>
-    </row>
-    <row r="226" spans="1:3">
+      <c r="C225" s="87" t="s">
+        <v>1386</v>
+      </c>
+      <c r="D225" s="51" t="s">
+        <v>944</v>
+      </c>
+      <c r="E225" s="53" t="s">
+        <v>1387</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H225" s="99" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" ht="60">
       <c r="A226" s="3">
         <v>3</v>
       </c>
       <c r="B226" s="3"/>
-      <c r="C226" s="80"/>
-    </row>
-    <row r="227" spans="1:3">
+      <c r="C226" s="87" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D226" s="51" t="s">
+        <v>1391</v>
+      </c>
+      <c r="E226" s="53" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F226" s="3" t="s">
+        <v>1388</v>
+      </c>
+      <c r="H226" s="99" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" ht="135">
       <c r="A227" s="3">
         <v>3</v>
       </c>
       <c r="B227" s="3"/>
-      <c r="C227" s="80"/>
-    </row>
-    <row r="228" spans="1:3">
+      <c r="C227" s="87" t="s">
+        <v>1390</v>
+      </c>
+      <c r="D227" s="51" t="s">
+        <v>944</v>
+      </c>
+      <c r="E227" s="53" t="s">
+        <v>1393</v>
+      </c>
+      <c r="F227" s="3" t="s">
+        <v>1394</v>
+      </c>
+      <c r="G227" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="H227" s="99" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" ht="30">
       <c r="A228" s="3">
         <v>3</v>
       </c>
       <c r="B228" s="3"/>
-      <c r="C228" s="80"/>
-    </row>
-    <row r="229" spans="1:3">
+      <c r="C228" s="87" t="s">
+        <v>1403</v>
+      </c>
+      <c r="D228" s="51" t="s">
+        <v>944</v>
+      </c>
+      <c r="E228" s="53" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F228" s="3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H228" s="99" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" ht="30">
       <c r="A229" s="3">
         <v>3</v>
       </c>
       <c r="B229" s="3"/>
-      <c r="C229" s="80"/>
-    </row>
-    <row r="230" spans="1:3">
+      <c r="C229" s="87" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E229" s="53" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F229" s="3" t="s">
+        <v>1398</v>
+      </c>
+      <c r="H229" s="99"/>
+    </row>
+    <row r="230" spans="1:8" ht="30">
       <c r="A230" s="3">
         <v>3</v>
       </c>
       <c r="B230" s="3"/>
-      <c r="C230" s="80"/>
-    </row>
-    <row r="231" spans="1:3">
+      <c r="C230" s="87" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E230" s="53" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F230" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="H230" s="99"/>
+    </row>
+    <row r="231" spans="1:8" ht="30">
       <c r="A231" s="3">
         <v>3</v>
       </c>
       <c r="B231" s="3"/>
-      <c r="C231" s="80"/>
-    </row>
-    <row r="232" spans="1:3">
+      <c r="C231" s="87" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E231" s="53" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F231" s="3" t="s">
+        <v>1400</v>
+      </c>
+      <c r="H231" s="99"/>
+    </row>
+    <row r="232" spans="1:8" ht="30">
       <c r="A232" s="3">
         <v>3</v>
       </c>
       <c r="B232" s="3"/>
-      <c r="C232" s="80"/>
-    </row>
-    <row r="233" spans="1:3">
+      <c r="C232" s="87" t="s">
+        <v>1403</v>
+      </c>
+      <c r="E232" s="53" t="s">
+        <v>1356</v>
+      </c>
+      <c r="F232" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="H232" s="99"/>
+    </row>
+    <row r="233" spans="1:8">
       <c r="A233" s="3">
         <v>3</v>
       </c>
       <c r="B233" s="3"/>
       <c r="C233" s="80"/>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:8">
       <c r="A234" s="3">
         <v>3</v>
       </c>
       <c r="B234" s="3"/>
       <c r="C234" s="80"/>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:8">
       <c r="A235" s="3">
         <v>3</v>
       </c>
       <c r="B235" s="3"/>
       <c r="C235" s="80"/>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:8">
       <c r="A236" s="3">
         <v>3</v>
       </c>
       <c r="B236" s="3"/>
       <c r="C236" s="80"/>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:8">
       <c r="A237" s="3">
         <v>3</v>
       </c>
       <c r="B237" s="3"/>
       <c r="C237" s="80"/>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:8">
       <c r="A238" s="3">
         <v>3</v>
       </c>
       <c r="B238" s="3"/>
       <c r="C238" s="80"/>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:8">
       <c r="A239" s="3">
         <v>3</v>
       </c>
       <c r="B239" s="3"/>
       <c r="C239" s="80"/>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:8">
       <c r="A240" s="3">
         <v>3</v>
       </c>
@@ -27275,8 +28527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C80C63-9F14-4F36-AB3C-26E3A4A9F7FA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD54" sqref="AD54"/>
+    <sheetView tabSelected="1" topLeftCell="E100" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X141" sqref="X141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>